<commit_message>
additional single annotated files added
</commit_message>
<xml_diff>
--- a/data/additional/single_annotated/full_fict/txt/metadata.xlsx
+++ b/data/additional/single_annotated/full_fict/txt/metadata.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github_Redewiedergabe\corpus\data\additional\single_annotated\full_fict\txt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub_RW\corpus\data\additional\single_annotated\full_fict\xmi\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BCC09A3-C7CF-45E5-B944-07FF0146840A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-27555" yWindow="495" windowWidth="27450" windowHeight="15330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="117">
   <si>
     <t>file</t>
   </si>
@@ -51,9 +52,6 @@
     <t>text_type</t>
   </si>
   <si>
-    <t>periodical</t>
-  </si>
-  <si>
     <t>narrative</t>
   </si>
   <si>
@@ -78,6 +76,9 @@
     <t>rwz_full_digbib_1208.xmi</t>
   </si>
   <si>
+    <t>rwz_full_digbib_1340.xmi</t>
+  </si>
+  <si>
     <t>rwz_full_digbib_2473.xmi</t>
   </si>
   <si>
@@ -123,6 +124,9 @@
     <t>neptune</t>
   </si>
   <si>
+    <t>uranus</t>
+  </si>
+  <si>
     <t>venus</t>
   </si>
   <si>
@@ -135,6 +139,9 @@
     <t>Heyking,_Elisabeth_von_Gewesen.tg75_1.xml</t>
   </si>
   <si>
+    <t>Keller,_Gottfried_Kleider_machen_Leute.tg808_1.xml</t>
+  </si>
+  <si>
     <t>Poe,_Edgar_Allan_Hinab_in_den_Maelstroem.tg46_1.xml</t>
   </si>
   <si>
@@ -165,6 +172,9 @@
     <t>1905</t>
   </si>
   <si>
+    <t>1874</t>
+  </si>
+  <si>
     <t>1841</t>
   </si>
   <si>
@@ -207,15 +217,15 @@
     <t>1900</t>
   </si>
   <si>
+    <t>1870</t>
+  </si>
+  <si>
     <t>1910</t>
   </si>
   <si>
     <t>1860</t>
   </si>
   <si>
-    <t>1870</t>
-  </si>
-  <si>
     <t>1820</t>
   </si>
   <si>
@@ -234,6 +244,9 @@
     <t>Gewesen</t>
   </si>
   <si>
+    <t>Kleider machen Leute</t>
+  </si>
+  <si>
     <t>Hinab in den Maelström</t>
   </si>
   <si>
@@ -285,6 +298,9 @@
     <t>Heyking, Elisabeth von</t>
   </si>
   <si>
+    <t>Keller, Gottfried</t>
+  </si>
+  <si>
     <t>Poe, Edgar Allan</t>
   </si>
   <si>
@@ -346,6 +362,9 @@
   </si>
   <si>
     <t>swiss</t>
+  </si>
+  <si>
+    <t>chevron</t>
   </si>
   <si>
     <t>ascii german</t>
@@ -357,7 +376,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -508,6 +527,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -543,6 +579,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -718,19 +771,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -776,807 +829,851 @@
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>16</v>
       </c>
       <c r="B2" t="s">
         <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="F2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="G2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="H2" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="I2" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="J2" t="s">
-        <v>102</v>
-      </c>
-      <c r="L2" t="s">
-        <v>101</v>
-      </c>
-      <c r="M2">
+        <v>107</v>
+      </c>
+      <c r="K2" t="s">
+        <v>106</v>
+      </c>
+      <c r="L2">
         <v>20124</v>
       </c>
+      <c r="M2" t="s">
+        <v>108</v>
+      </c>
       <c r="N2" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="O2" t="s">
-        <v>105</v>
-      </c>
-      <c r="P2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
         <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E3" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="F3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="G3" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="H3" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="I3" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="J3" t="s">
-        <v>102</v>
-      </c>
-      <c r="L3" t="s">
-        <v>101</v>
-      </c>
-      <c r="M3">
+        <v>107</v>
+      </c>
+      <c r="K3" t="s">
+        <v>106</v>
+      </c>
+      <c r="L3">
         <v>17966</v>
       </c>
+      <c r="M3" t="s">
+        <v>108</v>
+      </c>
       <c r="N3" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="O3" t="s">
-        <v>106</v>
-      </c>
-      <c r="P3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
         <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E4" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="F4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="G4" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="H4" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="I4" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="J4" t="s">
-        <v>102</v>
-      </c>
-      <c r="L4" t="s">
-        <v>101</v>
-      </c>
-      <c r="M4">
+        <v>107</v>
+      </c>
+      <c r="K4" t="s">
+        <v>106</v>
+      </c>
+      <c r="L4">
         <v>6423</v>
       </c>
+      <c r="M4" t="s">
+        <v>108</v>
+      </c>
       <c r="N4" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="O4" t="s">
-        <v>105</v>
-      </c>
-      <c r="P4" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
         <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D5" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E5" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="F5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G5" t="s">
+        <v>74</v>
+      </c>
+      <c r="H5" t="s">
+        <v>92</v>
+      </c>
+      <c r="I5" t="s">
+        <v>106</v>
+      </c>
+      <c r="J5" t="s">
+        <v>107</v>
+      </c>
+      <c r="K5" t="s">
+        <v>106</v>
+      </c>
+      <c r="L5">
+        <v>16635</v>
+      </c>
+      <c r="M5" t="s">
+        <v>108</v>
+      </c>
+      <c r="N5" t="s">
+        <v>110</v>
+      </c>
+      <c r="O5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" t="s">
+        <v>70</v>
+      </c>
+      <c r="G6" t="s">
+        <v>75</v>
+      </c>
+      <c r="H6" t="s">
+        <v>93</v>
+      </c>
+      <c r="I6" t="s">
+        <v>106</v>
+      </c>
+      <c r="J6" t="s">
+        <v>107</v>
+      </c>
+      <c r="K6" t="s">
+        <v>106</v>
+      </c>
+      <c r="L6">
+        <v>7288</v>
+      </c>
+      <c r="M6" t="s">
+        <v>108</v>
+      </c>
+      <c r="N6" t="s">
+        <v>111</v>
+      </c>
+      <c r="O6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F7" t="s">
+        <v>70</v>
+      </c>
+      <c r="G7" t="s">
+        <v>76</v>
+      </c>
+      <c r="H7" t="s">
+        <v>94</v>
+      </c>
+      <c r="I7" t="s">
+        <v>106</v>
+      </c>
+      <c r="J7" t="s">
+        <v>107</v>
+      </c>
+      <c r="K7" t="s">
+        <v>106</v>
+      </c>
+      <c r="L7">
+        <v>7066</v>
+      </c>
+      <c r="M7" t="s">
+        <v>108</v>
+      </c>
+      <c r="N7" t="s">
+        <v>112</v>
+      </c>
+      <c r="O7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" t="s">
         <v>67</v>
       </c>
-      <c r="G5" t="s">
-        <v>71</v>
-      </c>
-      <c r="H5" t="s">
-        <v>88</v>
-      </c>
-      <c r="I5" t="s">
-        <v>101</v>
-      </c>
-      <c r="J5" t="s">
-        <v>102</v>
-      </c>
-      <c r="L5" t="s">
-        <v>101</v>
-      </c>
-      <c r="M5">
-        <v>7288</v>
-      </c>
-      <c r="N5" t="s">
-        <v>103</v>
-      </c>
-      <c r="O5" t="s">
-        <v>106</v>
-      </c>
-      <c r="P5" t="s">
+      <c r="F8" t="s">
+        <v>70</v>
+      </c>
+      <c r="G8" t="s">
+        <v>77</v>
+      </c>
+      <c r="H8" t="s">
+        <v>95</v>
+      </c>
+      <c r="I8" t="s">
+        <v>106</v>
+      </c>
+      <c r="J8" t="s">
+        <v>107</v>
+      </c>
+      <c r="K8" t="s">
+        <v>106</v>
+      </c>
+      <c r="L8">
+        <v>9640</v>
+      </c>
+      <c r="M8" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" t="s">
-        <v>49</v>
-      </c>
-      <c r="E6" t="s">
-        <v>62</v>
-      </c>
-      <c r="F6" t="s">
-        <v>67</v>
-      </c>
-      <c r="G6" t="s">
-        <v>72</v>
-      </c>
-      <c r="H6" t="s">
-        <v>89</v>
-      </c>
-      <c r="I6" t="s">
-        <v>101</v>
-      </c>
-      <c r="J6" t="s">
-        <v>102</v>
-      </c>
-      <c r="L6" t="s">
-        <v>101</v>
-      </c>
-      <c r="M6">
-        <v>7066</v>
-      </c>
-      <c r="N6" t="s">
-        <v>103</v>
-      </c>
-      <c r="O6" t="s">
-        <v>107</v>
-      </c>
-      <c r="P6" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" t="s">
-        <v>50</v>
-      </c>
-      <c r="E7" t="s">
-        <v>63</v>
-      </c>
-      <c r="F7" t="s">
-        <v>67</v>
-      </c>
-      <c r="G7" t="s">
-        <v>73</v>
-      </c>
-      <c r="H7" t="s">
-        <v>90</v>
-      </c>
-      <c r="I7" t="s">
-        <v>101</v>
-      </c>
-      <c r="J7" t="s">
-        <v>102</v>
-      </c>
-      <c r="L7" t="s">
-        <v>101</v>
-      </c>
-      <c r="M7">
-        <v>9640</v>
-      </c>
-      <c r="N7" t="s">
-        <v>103</v>
-      </c>
-      <c r="O7" t="s">
-        <v>105</v>
-      </c>
-      <c r="P7" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="N8" t="s">
+        <v>110</v>
+      </c>
+      <c r="O8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>22</v>
-      </c>
-      <c r="B8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E8" t="s">
-        <v>64</v>
-      </c>
-      <c r="F8" t="s">
-        <v>67</v>
-      </c>
-      <c r="G8" t="s">
-        <v>74</v>
-      </c>
-      <c r="H8" t="s">
-        <v>91</v>
-      </c>
-      <c r="I8" t="s">
-        <v>101</v>
-      </c>
-      <c r="J8" t="s">
-        <v>102</v>
-      </c>
-      <c r="L8" t="s">
-        <v>101</v>
-      </c>
-      <c r="M8">
-        <v>10075</v>
-      </c>
-      <c r="N8" t="s">
-        <v>104</v>
-      </c>
-      <c r="O8" t="s">
-        <v>106</v>
-      </c>
-      <c r="P8" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>23</v>
       </c>
       <c r="B9" t="s">
         <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D9" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E9" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F9" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="G9" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="H9" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="I9" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="J9" t="s">
-        <v>102</v>
-      </c>
-      <c r="L9" t="s">
-        <v>101</v>
-      </c>
-      <c r="M9">
-        <v>11447</v>
+        <v>107</v>
+      </c>
+      <c r="K9" t="s">
+        <v>106</v>
+      </c>
+      <c r="L9">
+        <v>10075</v>
+      </c>
+      <c r="M9" t="s">
+        <v>109</v>
       </c>
       <c r="N9" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="O9" t="s">
-        <v>105</v>
-      </c>
-      <c r="P9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
         <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D10" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="E10" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="F10" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="G10" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="H10" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="I10" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="J10" t="s">
-        <v>102</v>
-      </c>
-      <c r="L10" t="s">
-        <v>101</v>
-      </c>
-      <c r="M10">
-        <v>8125</v>
+        <v>107</v>
+      </c>
+      <c r="K10" t="s">
+        <v>106</v>
+      </c>
+      <c r="L10">
+        <v>11447</v>
+      </c>
+      <c r="M10" t="s">
+        <v>108</v>
       </c>
       <c r="N10" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="O10" t="s">
-        <v>105</v>
-      </c>
-      <c r="P10" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
         <v>33</v>
       </c>
       <c r="C11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F11" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="G11" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="H11" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="I11" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="J11" t="s">
-        <v>102</v>
-      </c>
-      <c r="L11" t="s">
-        <v>101</v>
-      </c>
-      <c r="M11">
-        <v>10809</v>
+        <v>107</v>
+      </c>
+      <c r="K11" t="s">
+        <v>106</v>
+      </c>
+      <c r="L11">
+        <v>8125</v>
+      </c>
+      <c r="M11" t="s">
+        <v>108</v>
       </c>
       <c r="N11" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="O11" t="s">
-        <v>106</v>
-      </c>
-      <c r="P11" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" t="s">
         <v>33</v>
       </c>
       <c r="C12" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E12" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="F12" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="G12" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="H12" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="I12" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="J12" t="s">
-        <v>102</v>
-      </c>
-      <c r="L12" t="s">
-        <v>101</v>
-      </c>
-      <c r="M12">
-        <v>16798</v>
+        <v>107</v>
+      </c>
+      <c r="K12" t="s">
+        <v>106</v>
+      </c>
+      <c r="L12">
+        <v>10809</v>
+      </c>
+      <c r="M12" t="s">
+        <v>108</v>
       </c>
       <c r="N12" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="O12" t="s">
-        <v>105</v>
-      </c>
-      <c r="P12" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
         <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D13" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E13" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="F13" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="G13" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="H13" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="I13" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="J13" t="s">
-        <v>102</v>
-      </c>
-      <c r="L13" t="s">
-        <v>101</v>
-      </c>
-      <c r="M13">
-        <v>18447</v>
+        <v>107</v>
+      </c>
+      <c r="K13" t="s">
+        <v>106</v>
+      </c>
+      <c r="L13">
+        <v>16798</v>
+      </c>
+      <c r="M13" t="s">
+        <v>108</v>
       </c>
       <c r="N13" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="O13" t="s">
-        <v>105</v>
-      </c>
-      <c r="P13" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" t="s">
         <v>33</v>
       </c>
       <c r="C14" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D14" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E14" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F14" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="G14" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="H14" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="I14" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="J14" t="s">
-        <v>102</v>
-      </c>
-      <c r="L14" t="s">
-        <v>101</v>
-      </c>
-      <c r="M14">
-        <v>23856</v>
+        <v>107</v>
+      </c>
+      <c r="K14" t="s">
+        <v>106</v>
+      </c>
+      <c r="L14">
+        <v>18447</v>
+      </c>
+      <c r="M14" t="s">
+        <v>109</v>
       </c>
       <c r="N14" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="O14" t="s">
-        <v>105</v>
-      </c>
-      <c r="P14" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
         <v>33</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D15" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E15" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F15" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="G15" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="H15" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="I15" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="J15" t="s">
-        <v>102</v>
-      </c>
-      <c r="L15" t="s">
-        <v>101</v>
-      </c>
-      <c r="M15">
-        <v>10754</v>
+        <v>107</v>
+      </c>
+      <c r="K15" t="s">
+        <v>106</v>
+      </c>
+      <c r="L15">
+        <v>23856</v>
+      </c>
+      <c r="M15" t="s">
+        <v>108</v>
       </c>
       <c r="N15" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="O15" t="s">
-        <v>105</v>
-      </c>
-      <c r="P15" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B16" t="s">
         <v>33</v>
       </c>
       <c r="C16" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D16" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E16" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="F16" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="G16" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="H16" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="I16" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="J16" t="s">
-        <v>102</v>
-      </c>
-      <c r="L16" t="s">
-        <v>101</v>
-      </c>
-      <c r="M16">
-        <v>19008</v>
+        <v>107</v>
+      </c>
+      <c r="K16" t="s">
+        <v>106</v>
+      </c>
+      <c r="L16">
+        <v>10754</v>
+      </c>
+      <c r="M16" t="s">
+        <v>108</v>
       </c>
       <c r="N16" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="O16" t="s">
-        <v>105</v>
-      </c>
-      <c r="P16" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B17" t="s">
         <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D17" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E17" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="F17" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="G17" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H17" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="I17" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="J17" t="s">
-        <v>102</v>
-      </c>
-      <c r="L17" t="s">
-        <v>101</v>
-      </c>
-      <c r="M17">
-        <v>11429</v>
+        <v>107</v>
+      </c>
+      <c r="K17" t="s">
+        <v>106</v>
+      </c>
+      <c r="L17">
+        <v>19008</v>
+      </c>
+      <c r="M17" t="s">
+        <v>108</v>
       </c>
       <c r="N17" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="O17" t="s">
-        <v>107</v>
-      </c>
-      <c r="P17" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B18" t="s">
         <v>33</v>
       </c>
       <c r="C18" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D18" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E18" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="F18" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="G18" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="H18" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="I18" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="J18" t="s">
-        <v>102</v>
-      </c>
-      <c r="L18" t="s">
-        <v>101</v>
-      </c>
-      <c r="M18">
+        <v>107</v>
+      </c>
+      <c r="K18" t="s">
+        <v>106</v>
+      </c>
+      <c r="L18">
+        <v>11429</v>
+      </c>
+      <c r="M18" t="s">
+        <v>108</v>
+      </c>
+      <c r="N18" t="s">
+        <v>112</v>
+      </c>
+      <c r="O18" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" t="s">
+        <v>62</v>
+      </c>
+      <c r="E19" t="s">
+        <v>69</v>
+      </c>
+      <c r="F19" t="s">
+        <v>70</v>
+      </c>
+      <c r="G19" t="s">
+        <v>88</v>
+      </c>
+      <c r="H19" t="s">
+        <v>105</v>
+      </c>
+      <c r="I19" t="s">
+        <v>106</v>
+      </c>
+      <c r="J19" t="s">
+        <v>107</v>
+      </c>
+      <c r="K19" t="s">
+        <v>106</v>
+      </c>
+      <c r="L19">
         <v>9685</v>
       </c>
-      <c r="N18" t="s">
-        <v>103</v>
-      </c>
-      <c r="O18" t="s">
-        <v>105</v>
-      </c>
-      <c r="P18" t="s">
-        <v>109</v>
+      <c r="M19" t="s">
+        <v>108</v>
+      </c>
+      <c r="N19" t="s">
+        <v>110</v>
+      </c>
+      <c r="O19" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>